<commit_message>
Add some python sample codes
</commit_message>
<xml_diff>
--- a/python/03-excel/0301.xlsx
+++ b/python/03-excel/0301.xlsx
@@ -92,13 +92,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="yyyy\-m\-d"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="178" formatCode="[$￥-804]0.00"/>
+    <numFmt numFmtId="177" formatCode="[$￥-804]0.00"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="180" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="182" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -116,23 +116,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -143,9 +137,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -159,6 +167,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -168,18 +184,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -193,9 +201,32 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -228,37 +259,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
@@ -293,181 +293,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,8 +589,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -600,6 +600,30 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,26 +643,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -655,31 +670,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -688,148 +688,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -852,7 +852,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -864,7 +864,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -876,10 +876,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1239,10 +1239,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+            <a:latin typeface="Helvetica Neue Medium" panose="02000503000000020004"/>
+            <a:ea typeface="Helvetica Neue Medium" panose="02000503000000020004"/>
+            <a:cs typeface="Helvetica Neue Medium" panose="02000503000000020004"/>
+            <a:sym typeface="Helvetica Neue Medium" panose="02000503000000020004"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>